<commit_message>
Content for Week 2 Epi Cartography 1. Also updates to appendices on sf, tmap
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>module</t>
   </si>
@@ -44,9 +44,6 @@
     <t>A reference system that uses latitude and longitude to define the locations of points on the surface of a sphere or spheroid. A geographic coordinate system definition includes a datum, prime meridian, and angular unit</t>
   </si>
   <si>
-    <t>Attribute data</t>
-  </si>
-  <si>
     <t>Nonspatial information about a geographic feature in a GIS, usually stored in a table and linked to the feature by a unique identifier. For example, attributes of a county might include the population size, density, and birth rate for the resident population</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>Spatial data model: vector</t>
   </si>
   <si>
-    <t>Geometry data</t>
-  </si>
-  <si>
     <t>Term</t>
   </si>
   <si>
@@ -81,6 +75,60 @@
   </si>
   <si>
     <t>Spatial information about a geogrpahic feature. This could include the x, y coordinates for points or for vertices of lines or polygons, or the cell coordinates for raster data</t>
+  </si>
+  <si>
+    <t>Cartography</t>
+  </si>
+  <si>
+    <t>The production of maps, including construction of projections, design, compilation, drafting, and reproduction</t>
+  </si>
+  <si>
+    <t>Choropleth map</t>
+  </si>
+  <si>
+    <t>Isopleth map</t>
+  </si>
+  <si>
+    <t>A type of thematic map in which areas are shaded or patterned in proportion to a statistical variable that represents an aggregate summary of a geographic characteristic within each area, such as population density, disease risk, or standardized mortality ratio</t>
+  </si>
+  <si>
+    <t>A type of thematic map that uses contour lines or colors to indicate areas with similar regional aspects. It typically symbolizes the underlying statistic as varying continuously in space, in contrast to the discrete unit-specific variation of choropleth maps</t>
+  </si>
+  <si>
+    <t>Standardize Morbidity/Mortality Ratio (SMR)</t>
+  </si>
+  <si>
+    <t>The ratio of observed to expected disease morbidity or mortality. Often the 'expected' is defined as the overall population (or study-specific) rate; in that case the SMR indicates the relative deviation of a specific unit from the global or overall rate</t>
+  </si>
+  <si>
+    <t>Color palette: sequential</t>
+  </si>
+  <si>
+    <t>Color palette: diverging</t>
+  </si>
+  <si>
+    <t>Diverging schemes allow the emphasis of a quantitative data display to be progressions outward from a critical midpoint of the data range. A typical diverging scheme pairs sequential schemes based on two different hues so that they diverge from a shared light color, for the critical midpoint, toward dark colors of different hues at each extreme</t>
+  </si>
+  <si>
+    <t>Sequential data classes are logically arranged from high to low, and this stepped sequence of categories should be represented by sequential lightness steps. Low data values are usually represented by light colors and high values represented by dark colors. Transitions between hues may be used in a sequential scheme, but the light-to-dark progression should dominate the scheme.</t>
+  </si>
+  <si>
+    <t>Qualitative schemes use differences in hue to represent nominal differences, or differences in kind. The lightness of the hues used for qualitative categories should be similar but not equal. </t>
+  </si>
+  <si>
+    <t>Color palette: qualitative</t>
+  </si>
+  <si>
+    <t>Visual hierarchy</t>
+  </si>
+  <si>
+    <t>The apparent order of importance of phenomena perceived by the human eye.  In cartography, this principle is a fundamental part of map composition; since the goal of map composition is to clearly convey a desired purpose, the attention of readers should be focused on the map elements that are most relevant to the purpose.</t>
+  </si>
+  <si>
+    <t>Data, attribute</t>
+  </si>
+  <si>
+    <t>Data, geometry</t>
   </si>
 </sst>
 </file>
@@ -398,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,10 +462,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -436,10 +484,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -447,10 +495,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -458,10 +506,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -472,7 +520,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -491,10 +539,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
         <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -502,10 +550,98 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>11</v>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update EPI Cartography 2; add license info
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>module</t>
   </si>
@@ -129,6 +129,42 @@
   </si>
   <si>
     <t>Data, geometry</t>
+  </si>
+  <si>
+    <t>Confidentiality</t>
+  </si>
+  <si>
+    <t>Privacy</t>
+  </si>
+  <si>
+    <t>Belmont principles: justice</t>
+  </si>
+  <si>
+    <t>Belmont principles: respect for persons</t>
+  </si>
+  <si>
+    <t>Belmont principles: beneficence</t>
+  </si>
+  <si>
+    <t>Geomask</t>
+  </si>
+  <si>
+    <t>Defined by two ethical convictions: a) individuals should be treated as autonomous agents; b) persons with diminished autonomy are entitled to protection</t>
+  </si>
+  <si>
+    <t>Ethical principle that the burdens and benefits of research and public health practice should be justly distributed, including attention to need, effort, contribution, and merit</t>
+  </si>
+  <si>
+    <t>The right of an individual to keep his or her information (health related or otherwise) private</t>
+  </si>
+  <si>
+    <t>The duty of anyone entrusted with health information to keep that information private</t>
+  </si>
+  <si>
+    <t>Two general rules have been formulated as complementary expressions of beneficent actions in this sense: (1) do not harm and (2) maximize possible benefits and minimize possible harms</t>
+  </si>
+  <si>
+    <t>A class of methods for changing the geographic location of an individual in an unpredictable way to protect confidentiality, while trying to preserve the relationship between geocoded locations and disease occurrence (Sherman and Fetters 2007, Wiggins 2002)</t>
   </si>
 </sst>
 </file>
@@ -446,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,6 +680,72 @@
         <v>32</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Disease Mapping 1 content added
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>module</t>
   </si>
@@ -137,15 +137,6 @@
     <t>Privacy</t>
   </si>
   <si>
-    <t>Belmont principles: justice</t>
-  </si>
-  <si>
-    <t>Belmont principles: respect for persons</t>
-  </si>
-  <si>
-    <t>Belmont principles: beneficence</t>
-  </si>
-  <si>
     <t>Geomask</t>
   </si>
   <si>
@@ -161,10 +152,55 @@
     <t>The duty of anyone entrusted with health information to keep that information private</t>
   </si>
   <si>
-    <t>Two general rules have been formulated as complementary expressions of beneficent actions in this sense: (1) do not harm and (2) maximize possible benefits and minimize possible harms</t>
-  </si>
-  <si>
     <t>A class of methods for changing the geographic location of an individual in an unpredictable way to protect confidentiality, while trying to preserve the relationship between geocoded locations and disease occurrence (Sherman and Fetters 2007, Wiggins 2002)</t>
+  </si>
+  <si>
+    <t>Ethical principles: respect for persons</t>
+  </si>
+  <si>
+    <t>Ethical principles: justice</t>
+  </si>
+  <si>
+    <t>Ethical principles: beneficence</t>
+  </si>
+  <si>
+    <t>Two general rules have been formulated as complementary expressions of beneficent actions in this sense: (1) do not harm (e.g. non-maleficence) and (2) maximize possible benefits and minimize possible harms</t>
+  </si>
+  <si>
+    <t>Spatial heterogeneity</t>
+  </si>
+  <si>
+    <t>Spatial dependence</t>
+  </si>
+  <si>
+    <t>Stationarity vs non-stationarity</t>
+  </si>
+  <si>
+    <t>Global vs Local spatial analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attributes or statistical parameters are varied (e.g. not homogenous) across sub-areas in a broader region. In Disease mapping we typically are evaluating whether (and how much) disease intensity (risk, rate, prevalence) varies across places. </t>
+  </si>
+  <si>
+    <t>When attribute values or statistical parameters are, on avreage, more similar for nearby places than they are for distant places. Spatial dependence is evaluated by looking at pairs or sets of places.</t>
+  </si>
+  <si>
+    <t>Many statistics assume that the parameter, estimate, or property is constant across sub-units. For example if we take the average height of a population, under stationarity we would assume that average applies equally to sub-populations. In contrast, non-stationarity implies the parameter, estimate, or property varies across sub-groups. In spatial analysis stationarity is an assumption of homogeneity, and non-stationarity allows for heterogeneity.</t>
+  </si>
+  <si>
+    <t>Empirical Bayes methods</t>
+  </si>
+  <si>
+    <t>Estimation procedures in a Bayesian framework in which the prior distribution is estimated from the data. In disease mapping, Empirical Bayes estimators use global or local disease information as a prior in estimating (and smoothing/stabilizing) each local rate</t>
+  </si>
+  <si>
+    <t>Bayesian methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methods of statistical inference in which Bayes' theorem is used to update the probability for a hypothesis as more evidence or information becomes available. In disease mapping, the Bayesian framework is frequently used to accomplish rate stabilization and smoothing by using global or local data to inform the 'prior' </t>
+  </si>
+  <si>
+    <t>Global analysis evaluates a pattern or trends that characterizes the entire study region; in contrast local analysis characterizes patterns that are unique to each sub-region of the study area</t>
   </si>
 </sst>
 </file>
@@ -482,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +724,7 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -699,7 +735,7 @@
         <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -707,10 +743,10 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
         <v>38</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -718,10 +754,10 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -729,10 +765,10 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -740,10 +776,87 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Disease Mapping 2 content; fix small error sin Disease Mapping 1
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>module</t>
   </si>
@@ -201,6 +201,48 @@
   </si>
   <si>
     <t>Global analysis evaluates a pattern or trends that characterizes the entire study region; in contrast local analysis characterizes patterns that are unique to each sub-region of the study area</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>A fundamental dimension in geography referring to the strength of connectedness or proximity in eculidean space, social space, or network space. Distance if fundamental because we assume that a) entities that are closer are, on average, more alike than entities that are far apart; and b) increasing distance represents increasing friction or imedance to social and health-relevant interaction</t>
+  </si>
+  <si>
+    <t>Aspatial vs. Spatial</t>
+  </si>
+  <si>
+    <t>This distinction refers to whether or not spatial proximity or contiguity is explicitly incorporated into an analysis (spatial) versus whether spatial units are treated as independent of one another (aspatial)</t>
+  </si>
+  <si>
+    <t>Spatial neighbors</t>
+  </si>
+  <si>
+    <t>The set of spatial entities that are determined to be 'near' rather than 'far' (in binary terms) or relatively 'closer' or 'further' (in continuous terms). The definition of 'neighbors' is part of specifying spatial relatedness.</t>
+  </si>
+  <si>
+    <t>Spatial weights matrix</t>
+  </si>
+  <si>
+    <t>Typically a square matrix (n rows x n columns where n=geographic units) indexing all units on rows and columns. The values in the matrix indicate the spatial connectedness between all pairs of units.</t>
+  </si>
+  <si>
+    <t>Neighbor symmetry</t>
+  </si>
+  <si>
+    <t>An attribute of spatial relationships in which it is assumed that if spatial unit A is a neighbor with B, then spatial unit B is also a neighbor with A. Some neighbor definitions (e.g. k-nearest neighbors) do not require symmetry.</t>
+  </si>
+  <si>
+    <t>Toblers' First Law of Geography</t>
+  </si>
+  <si>
+    <t>All things are related, but near things are more related on average than distant things</t>
+  </si>
+  <si>
+    <t>Delauney triangulation</t>
+  </si>
+  <si>
+    <t>Geometric strategy for creating a mesh of contiguous, nonoverlapping triangles from a dataset of points. If points are the centroids of polygons, the triangle edges become graph-based definitions of spatial neighbors</t>
   </si>
 </sst>
 </file>
@@ -236,8 +278,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,6 +902,83 @@
         <v>55</v>
       </c>
     </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Push Disease Mapping 3, as well as minor changes to 2 and elsewhere
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>module</t>
   </si>
@@ -243,6 +243,60 @@
   </si>
   <si>
     <t>Geometric strategy for creating a mesh of contiguous, nonoverlapping triangles from a dataset of points. If points are the centroids of polygons, the triangle edges become graph-based definitions of spatial neighbors</t>
+  </si>
+  <si>
+    <t>Spatial intensity</t>
+  </si>
+  <si>
+    <t>A measure of the ratio of events at specific points to a unit of area. Spatial intensity describes the spatially continuous surface of event occurrence. In kernel density estimation, a spatial intensity surface integrates (or sums) to the sample size across a study region.</t>
+  </si>
+  <si>
+    <t>Spatial density</t>
+  </si>
+  <si>
+    <t>A standardized metric of spatial intensity. Related to a probability density function, it is a proportionate indicator of how much of the total events occur in a specific region. In kernel density estimation, the density surface integrates (or sums) to 1 across a study region.</t>
+  </si>
+  <si>
+    <t>Bandwidth</t>
+  </si>
+  <si>
+    <t>A measure of the width or spatial extent of a two-dimensional kernel density estimator. The bandwidth is the key to controlling how much smoothing occurs, with larger bandwidths producing more smooth surfaces, and smaller bandwidths producing less smooth surfaces</t>
+  </si>
+  <si>
+    <t>Geographic-weighting</t>
+  </si>
+  <si>
+    <t>Kernel density estimator</t>
+  </si>
+  <si>
+    <t>A non-parametric way to estimate the probability distribution function of a random variable. In spatial (e.g. 2-d) kernel density estimation, it is a way to describe the spatially continuous variation in the intensity of events (points).</t>
+  </si>
+  <si>
+    <t>A method for calculating summary weighted statistics by relying on a kernel density estimator to describe the weights in local summaries.</t>
+  </si>
+  <si>
+    <t>Homogenous Poisson Point Process</t>
+  </si>
+  <si>
+    <t>A spatial statistical assumption that the count of events in an arbitrarily small area is distributed Poisson with mean lambda for all regions</t>
+  </si>
+  <si>
+    <t>Inhomogenous Poisson Point Process</t>
+  </si>
+  <si>
+    <t>A spatial statistical assumption that the count of events in an arbitrarily small area is distributed Poisson with mean lambda that varies through space as a function of the underlying population at risk. This is true for most spatial epidemiology.</t>
+  </si>
+  <si>
+    <t>Bandwidth, fixed</t>
+  </si>
+  <si>
+    <t>A fixed bandwidth means the width or search radius of the spatial kernel density estimator is constant (fixed) for the full study region</t>
+  </si>
+  <si>
+    <t>Bandwidth, adaptive</t>
+  </si>
+  <si>
+    <t>An adaptive bandwith means the width or search radius of the spatial kernel density estimator varies or adapts through space, usually to maintain a constant number of points within the window. The result is that in areas with few points there is more smoothing, whereas in areas with many points there is more granularity</t>
   </si>
 </sst>
 </file>
@@ -561,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,6 +1033,105 @@
         <v>72</v>
       </c>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Disease Mapping IV; minor edits to DM 2-3
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
   <si>
     <t>module</t>
   </si>
@@ -297,6 +297,36 @@
   </si>
   <si>
     <t>An adaptive bandwith means the width or search radius of the spatial kernel density estimator varies or adapts through space, usually to maintain a constant number of points within the window. The result is that in areas with few points there is more smoothing, whereas in areas with many points there is more granularity</t>
+  </si>
+  <si>
+    <t>Inference in a frequentist framework draws conclusions from sample data by conceiving of this specific 'experiment' or sample as only one of thousands of possible experiments/samples, each capable of producing statistically independent results. Thus our inference is based on the probability of a given parameter (e.g. from one sample or experiment) arising in relation to all other (random) possibilities.</t>
+  </si>
+  <si>
+    <t>Bayesian Inference</t>
+  </si>
+  <si>
+    <t>Frequentist Inference</t>
+  </si>
+  <si>
+    <t>Bayesian is a process of using observed data to update prior beliefs. Typically parameters are assumed to be random variables arising from a distribution (e.g. rather than a discrete and solitary truth).</t>
+  </si>
+  <si>
+    <t>Prior</t>
+  </si>
+  <si>
+    <t>In Bayesian inference, the 'prior' is a formalized statement of the probability of a parameter, as stated before we see the data.</t>
+  </si>
+  <si>
+    <t>Posterior</t>
+  </si>
+  <si>
+    <t>In Bayesian inference, the 'posterior' is a formalized statement about the updated belief of the value of a parameter, conditional on the data (the likelihood) and the prior.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conditional auto-regressive (CAR) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The CAR is a common prior for spatial disease mapping, particularly in a Bayesian framework. A CAR prior suggests that the value for a given area can be estimated CONDITIONAL ON the level of neighboring values. </t>
   </si>
 </sst>
 </file>
@@ -615,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,6 +1162,61 @@
         <v>90</v>
       </c>
     </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>7</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>7</v>
+      </c>
+      <c r="B49" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Spatial structure 1, plus some minor tweaks to disease mapping
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
   <si>
     <t>module</t>
   </si>
@@ -327,6 +327,36 @@
   </si>
   <si>
     <t xml:space="preserve">The CAR is a common prior for spatial disease mapping, particularly in a Bayesian framework. A CAR prior suggests that the value for a given area can be estimated CONDITIONAL ON the level of neighboring values. </t>
+  </si>
+  <si>
+    <t>1st order process</t>
+  </si>
+  <si>
+    <t>2nd order process</t>
+  </si>
+  <si>
+    <t>Statistical measures where units taken one at a time. Spatial heterogeneity is about how the mean intensity varies for each unit, and is therefore primarily about first order process</t>
+  </si>
+  <si>
+    <t>Statistical measures where units considered at least two at a time. Spatial dependence is about correlation or relatedness between units and is therefore about 2nd order processes</t>
+  </si>
+  <si>
+    <t>Spatial dependence: Global</t>
+  </si>
+  <si>
+    <t>Evaluation of whether, on average, there is spatial independence (null) or spatial dependence (alternative) in a dataset. A global test returns a single test statistic for the entire dataset</t>
+  </si>
+  <si>
+    <t>Spatial dependence: Local</t>
+  </si>
+  <si>
+    <t>Evaluation of place-specific dependence by comparing, for each region, the correlation between the index value and the value of the neighbors. Local tests result in a stest statistic for each and every region</t>
+  </si>
+  <si>
+    <t>Spatial dependence: Focal</t>
+  </si>
+  <si>
+    <t>Evaluation of clustering or dependence of events or values in a specific focal area, typically defined in relation to a putative hazard</t>
   </si>
 </sst>
 </file>
@@ -645,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,6 +1247,83 @@
         <v>100</v>
       </c>
     </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>8</v>
+      </c>
+      <c r="B52" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>8</v>
+      </c>
+      <c r="B54" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>8</v>
+      </c>
+      <c r="B55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>8</v>
+      </c>
+      <c r="B57" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Week 9 cluster/structure 2 updates
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="113">
   <si>
     <t>module</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>Evaluation of clustering or dependence of events or values in a specific focal area, typically defined in relation to a putative hazard</t>
+  </si>
+  <si>
+    <t>Spatial scan statistic</t>
+  </si>
+  <si>
+    <t>A test for extreme or unusual event intensity inside versus outside a varying regional window, in an effort to detect local clusters of disease</t>
   </si>
 </sst>
 </file>
@@ -675,15 +681,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1324,6 +1330,72 @@
         <v>110</v>
       </c>
     </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>9</v>
+      </c>
+      <c r="B59" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>9</v>
+      </c>
+      <c r="B60" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>9</v>
+      </c>
+      <c r="B61" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>9</v>
+      </c>
+      <c r="B62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C62" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>9</v>
+      </c>
+      <c r="B63" t="s">
+        <v>48</v>
+      </c>
+      <c r="C63" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>9</v>
+      </c>
+      <c r="B64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add spatial regression 1
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
   <si>
     <t>module</t>
   </si>
@@ -363,6 +363,18 @@
   </si>
   <si>
     <t>A test for extreme or unusual event intensity inside versus outside a varying regional window, in an effort to detect local clusters of disease</t>
+  </si>
+  <si>
+    <t>Data generating process</t>
+  </si>
+  <si>
+    <t>The true underlying causal structure that gives rise to (generates) the data from which you sampled. The data generating process is not known. We use models to try to emulate or approximate the data generating process.</t>
+  </si>
+  <si>
+    <t>Model residual</t>
+  </si>
+  <si>
+    <t>The difference between the model predicted value of the outcomee and the observed value. In spatial epidemiology, model residuals can provide clues as to the presence of missing variables that produce spatial patterns</t>
   </si>
 </sst>
 </file>
@@ -681,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:A64"/>
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,6 +1408,28 @@
         <v>58</v>
       </c>
     </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>10</v>
+      </c>
+      <c r="B65" t="s">
+        <v>113</v>
+      </c>
+      <c r="C65" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>10</v>
+      </c>
+      <c r="B66" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Spatial Regression 2: GWR
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="120">
   <si>
     <t>module</t>
   </si>
@@ -375,6 +375,15 @@
   </si>
   <si>
     <t>The difference between the model predicted value of the outcomee and the observed value. In spatial epidemiology, model residuals can provide clues as to the presence of missing variables that produce spatial patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stationary' statistics are those for which the global value is true for all sub-groups (e.g. sub-population or places). In contrast, non-stationarity is when the value of a given statistic is not singularly global, but in fact depends on the sub-group (e.g. populatio or location). Spatia non-stationarity can refer to disease intensity (e.g. spatial heterogeneity) or to variable relationships (e.g. spatially varying coefficients). </t>
+  </si>
+  <si>
+    <t>Geographically weighted regression</t>
+  </si>
+  <si>
+    <t>A multivariable regression that is re-fit for multiple sub-regions within a study area, typically weighting the observations using a kernel density function. The goal of GWR is to identify statistical evidence for non-stationarity (e.g. does a locally varying regression fit the data better than a single global model, after penalizing for multiple comparisons?) and if present to quantify their values and spatial patterns.</t>
   </si>
 </sst>
 </file>
@@ -410,9 +419,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1430,6 +1440,61 @@
         <v>116</v>
       </c>
     </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>11</v>
+      </c>
+      <c r="B67" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>11</v>
+      </c>
+      <c r="B68" t="s">
+        <v>102</v>
+      </c>
+      <c r="C68" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>11</v>
+      </c>
+      <c r="B69" t="s">
+        <v>49</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>11</v>
+      </c>
+      <c r="B70" t="s">
+        <v>118</v>
+      </c>
+      <c r="C70" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>11</v>
+      </c>
+      <c r="B71" t="s">
+        <v>113</v>
+      </c>
+      <c r="C71" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
First commit 2021 with new bs4_book format
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkram02\Box\SpatialEpi-2020\EPI563-SpatialEPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkram02\OneDrive - Emory University\EPI563-Spatial Epi\SpatialEpi-2021\EPI563-SpatialEPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8376"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="133">
   <si>
     <t>module</t>
   </si>
@@ -417,6 +417,12 @@
   </si>
   <si>
     <t>The true underlying causal structure that gives rise to (generates) the data from which you sampled. The data generating process is not typically known. We use models to try to emulate or approximate the data generating process.</t>
+  </si>
+  <si>
+    <t>Geopackage</t>
+  </si>
+  <si>
+    <t>A data storage format suitable for containing vector or raster data in a compact and portable file. It is an alternative (and in my opinion a superior alternative!) to ESRI shapefiles.</t>
   </si>
 </sst>
 </file>
@@ -736,18 +742,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -758,7 +764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -769,7 +775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -780,7 +786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -791,7 +797,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -802,7 +808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -813,7 +819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -824,773 +830,784 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
       <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
         <v>37</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>4</v>
-      </c>
-      <c r="B24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>4</v>
       </c>
       <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
         <v>54</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>5</v>
-      </c>
-      <c r="B31" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>5</v>
       </c>
       <c r="B37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
         <v>71</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>6</v>
-      </c>
-      <c r="B38" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>6</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C44" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C45" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>6</v>
       </c>
       <c r="B46" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
         <v>89</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>7</v>
-      </c>
-      <c r="B47" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C48" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C50" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>7</v>
       </c>
       <c r="B51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
         <v>99</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>8</v>
-      </c>
-      <c r="B52" t="s">
-        <v>101</v>
-      </c>
-      <c r="C52" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C53" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="C54" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>48</v>
       </c>
       <c r="C56" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C57" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>8</v>
       </c>
       <c r="B58" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
         <v>109</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>9</v>
-      </c>
-      <c r="B59" t="s">
-        <v>101</v>
-      </c>
-      <c r="C59" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C60" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>9</v>
       </c>
       <c r="B61" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C61" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="C62" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C63" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>9</v>
       </c>
       <c r="B64" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>9</v>
+      </c>
+      <c r="B65" t="s">
         <v>50</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>10</v>
-      </c>
-      <c r="B65" t="s">
-        <v>113</v>
-      </c>
-      <c r="C65" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>10</v>
       </c>
       <c r="B66" t="s">
+        <v>113</v>
+      </c>
+      <c r="C66" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>10</v>
+      </c>
+      <c r="B67" t="s">
         <v>115</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>11</v>
-      </c>
-      <c r="B67" t="s">
-        <v>101</v>
-      </c>
-      <c r="C67" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C68" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>49</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="C69" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>118</v>
-      </c>
-      <c r="C70" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>11</v>
       </c>
       <c r="B71" t="s">
+        <v>118</v>
+      </c>
+      <c r="C71" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>11</v>
+      </c>
+      <c r="B72" t="s">
         <v>113</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>12</v>
-      </c>
-      <c r="B72" t="s">
-        <v>120</v>
-      </c>
-      <c r="C72" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C73" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>12</v>
       </c>
       <c r="B74" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C74" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C75" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>12</v>
       </c>
       <c r="B76" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C76" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>12</v>
       </c>
       <c r="B77" t="s">
+        <v>128</v>
+      </c>
+      <c r="C77" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>12</v>
+      </c>
+      <c r="B78" t="s">
         <v>113</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update to week 2 text, minor tweaks
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -107,9 +107,6 @@
     <t>Color palette: diverging</t>
   </si>
   <si>
-    <t>Diverging schemes allow the emphasis of a quantitative data display to be progressions outward from a critical midpoint of the data range. A typical diverging scheme pairs sequential schemes based on two different hues so that they diverge from a shared light color, for the critical midpoint, toward dark colors of different hues at each extreme</t>
-  </si>
-  <si>
     <t>Sequential data classes are logically arranged from high to low, and this stepped sequence of categories should be represented by sequential lightness steps. Low data values are usually represented by light colors and high values represented by dark colors. Transitions between hues may be used in a sequential scheme, but the light-to-dark progression should dominate the scheme.</t>
   </si>
   <si>
@@ -423,6 +420,9 @@
   </si>
   <si>
     <t>A data storage format suitable for containing vector or raster data in a compact and portable file. It is an alternative (and in my opinion a superior alternative!) to ESRI shapefiles.</t>
+  </si>
+  <si>
+    <t>Diverging schemes allow the emphasis of a quantitative data display that progresses outward from a critical midpoint of the data range. A typical diverging scheme pairs sequential schemes based on two different hues so that they diverge from a shared light color, for the critical midpoint, toward dark colors of different hues at each extreme</t>
   </si>
 </sst>
 </file>
@@ -745,7 +745,7 @@
   <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,7 +780,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -791,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -835,10 +835,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" t="s">
         <v>131</v>
-      </c>
-      <c r="C8" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -915,7 +915,7 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -926,7 +926,7 @@
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -934,10 +934,10 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -945,10 +945,10 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
         <v>31</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -956,10 +956,10 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -967,10 +967,10 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -978,10 +978,10 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -989,10 +989,10 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1000,10 +1000,10 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
         <v>45</v>
-      </c>
-      <c r="C23" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1011,10 +1011,10 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1022,10 +1022,10 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1033,10 +1033,10 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1044,10 +1044,10 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1055,10 +1055,10 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1077,10 +1077,10 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
         <v>56</v>
-      </c>
-      <c r="C30" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1088,10 +1088,10 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
         <v>54</v>
-      </c>
-      <c r="C31" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1099,10 +1099,10 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1110,10 +1110,10 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
         <v>61</v>
-      </c>
-      <c r="C33" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1121,10 +1121,10 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
         <v>63</v>
-      </c>
-      <c r="C34" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1132,10 +1132,10 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
         <v>65</v>
-      </c>
-      <c r="C35" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1143,10 +1143,10 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" t="s">
         <v>67</v>
-      </c>
-      <c r="C36" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1154,10 +1154,10 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" t="s">
         <v>69</v>
-      </c>
-      <c r="C37" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1165,10 +1165,10 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" t="s">
         <v>71</v>
-      </c>
-      <c r="C38" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1176,10 +1176,10 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" t="s">
         <v>73</v>
-      </c>
-      <c r="C39" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1187,10 +1187,10 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" t="s">
         <v>75</v>
-      </c>
-      <c r="C40" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1198,10 +1198,10 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" t="s">
         <v>77</v>
-      </c>
-      <c r="C41" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1209,10 +1209,10 @@
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1220,10 +1220,10 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" t="s">
         <v>80</v>
-      </c>
-      <c r="C43" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1231,10 +1231,10 @@
         <v>6</v>
       </c>
       <c r="B44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" t="s">
         <v>83</v>
-      </c>
-      <c r="C44" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1242,10 +1242,10 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" t="s">
         <v>85</v>
-      </c>
-      <c r="C45" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1253,10 +1253,10 @@
         <v>6</v>
       </c>
       <c r="B46" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" t="s">
         <v>87</v>
-      </c>
-      <c r="C46" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1264,10 +1264,10 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" t="s">
         <v>89</v>
-      </c>
-      <c r="C47" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1275,10 +1275,10 @@
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1286,10 +1286,10 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1297,10 +1297,10 @@
         <v>7</v>
       </c>
       <c r="B50" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" t="s">
         <v>95</v>
-      </c>
-      <c r="C50" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1308,10 +1308,10 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" t="s">
         <v>97</v>
-      </c>
-      <c r="C51" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1319,10 +1319,10 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" t="s">
         <v>99</v>
-      </c>
-      <c r="C52" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1330,10 +1330,10 @@
         <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1341,10 +1341,10 @@
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1352,10 +1352,10 @@
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1363,10 +1363,10 @@
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1374,10 +1374,10 @@
         <v>8</v>
       </c>
       <c r="B57" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" t="s">
         <v>105</v>
-      </c>
-      <c r="C57" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1385,10 +1385,10 @@
         <v>8</v>
       </c>
       <c r="B58" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" t="s">
         <v>107</v>
-      </c>
-      <c r="C58" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1396,10 +1396,10 @@
         <v>8</v>
       </c>
       <c r="B59" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" t="s">
         <v>109</v>
-      </c>
-      <c r="C59" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1407,10 +1407,10 @@
         <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C60" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1418,10 +1418,10 @@
         <v>9</v>
       </c>
       <c r="B61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1429,10 +1429,10 @@
         <v>9</v>
       </c>
       <c r="B62" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62" t="s">
         <v>111</v>
-      </c>
-      <c r="C62" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1440,10 +1440,10 @@
         <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1451,10 +1451,10 @@
         <v>9</v>
       </c>
       <c r="B64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1462,10 +1462,10 @@
         <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1473,10 +1473,10 @@
         <v>10</v>
       </c>
       <c r="B66" t="s">
+        <v>112</v>
+      </c>
+      <c r="C66" t="s">
         <v>113</v>
-      </c>
-      <c r="C66" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1484,10 +1484,10 @@
         <v>10</v>
       </c>
       <c r="B67" t="s">
+        <v>114</v>
+      </c>
+      <c r="C67" t="s">
         <v>115</v>
-      </c>
-      <c r="C67" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1495,10 +1495,10 @@
         <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C68" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1506,10 +1506,10 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C69" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1517,10 +1517,10 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1528,10 +1528,10 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
+        <v>117</v>
+      </c>
+      <c r="C71" t="s">
         <v>118</v>
-      </c>
-      <c r="C71" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -1539,10 +1539,10 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C72" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -1550,10 +1550,10 @@
         <v>12</v>
       </c>
       <c r="B73" t="s">
+        <v>119</v>
+      </c>
+      <c r="C73" t="s">
         <v>120</v>
-      </c>
-      <c r="C73" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -1561,10 +1561,10 @@
         <v>12</v>
       </c>
       <c r="B74" t="s">
+        <v>121</v>
+      </c>
+      <c r="C74" t="s">
         <v>122</v>
-      </c>
-      <c r="C74" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -1572,10 +1572,10 @@
         <v>12</v>
       </c>
       <c r="B75" t="s">
+        <v>123</v>
+      </c>
+      <c r="C75" t="s">
         <v>124</v>
-      </c>
-      <c r="C75" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1583,10 +1583,10 @@
         <v>12</v>
       </c>
       <c r="B76" t="s">
+        <v>125</v>
+      </c>
+      <c r="C76" t="s">
         <v>126</v>
-      </c>
-      <c r="C76" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -1594,10 +1594,10 @@
         <v>12</v>
       </c>
       <c r="B77" t="s">
+        <v>127</v>
+      </c>
+      <c r="C77" t="s">
         <v>128</v>
-      </c>
-      <c r="C77" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -1605,10 +1605,10 @@
         <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C78" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating Disease Mapping 3, 4
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8376"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="133">
   <si>
     <t>module</t>
   </si>
@@ -233,9 +233,6 @@
     <t>Toblers' First Law of Geography</t>
   </si>
   <si>
-    <t>All things are related, but near things are more related on average than distant things</t>
-  </si>
-  <si>
     <t>Delauney triangulation</t>
   </si>
   <si>
@@ -423,6 +420,9 @@
   </si>
   <si>
     <t>Diverging schemes allow the emphasis of a quantitative data display that progresses outward from a critical midpoint of the data range. A typical diverging scheme pairs sequential schemes based on two different hues so that they diverge from a shared light color, for the critical midpoint, toward dark colors of different hues at each extreme</t>
+  </si>
+  <si>
+    <t>All things are related, but near things are more related on average than distant things. Note that there is some debate about whether this statistical truism is a universal 'Law of Geography'. For example the ubiquitous correlation of spatially adjacent measures could occur for many non-causal reasons including confounding or selection.</t>
   </si>
 </sst>
 </file>
@@ -742,18 +742,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -764,7 +764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -775,7 +775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -786,7 +786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -797,7 +797,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -808,7 +808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -819,7 +819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -830,18 +830,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="s">
         <v>130</v>
       </c>
-      <c r="C8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -852,7 +852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -863,7 +863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -874,7 +874,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -885,7 +885,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -896,7 +896,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -907,7 +907,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -918,7 +918,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -926,10 +926,10 @@
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -940,7 +940,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -951,7 +951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
@@ -962,7 +962,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -973,7 +973,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -984,7 +984,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -995,7 +995,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5</v>
       </c>
@@ -1157,131 +1157,131 @@
         <v>68</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>5</v>
       </c>
       <c r="B38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" t="s">
         <v>70</v>
       </c>
-      <c r="C38" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>6</v>
       </c>
       <c r="B39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" t="s">
         <v>72</v>
       </c>
-      <c r="C39" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>6</v>
       </c>
       <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" t="s">
         <v>74</v>
       </c>
-      <c r="C40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6</v>
       </c>
       <c r="B41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" t="s">
         <v>76</v>
       </c>
-      <c r="C41" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>6</v>
       </c>
       <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" t="s">
         <v>79</v>
       </c>
-      <c r="C43" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>6</v>
       </c>
       <c r="B44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" t="s">
         <v>82</v>
       </c>
-      <c r="C44" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6</v>
       </c>
       <c r="B47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" t="s">
         <v>88</v>
       </c>
-      <c r="C47" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>7</v>
-      </c>
-      <c r="B48" t="s">
-        <v>92</v>
-      </c>
-      <c r="C48" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7</v>
       </c>
@@ -1289,326 +1289,337 @@
         <v>91</v>
       </c>
       <c r="C49" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C50" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C51" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>7</v>
       </c>
       <c r="B52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>7</v>
+      </c>
+      <c r="B53" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" t="s">
         <v>98</v>
       </c>
-      <c r="C52" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <v>8</v>
-      </c>
-      <c r="B53" t="s">
-        <v>100</v>
-      </c>
-      <c r="C53" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>8</v>
       </c>
       <c r="B54" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" t="s">
         <v>101</v>
       </c>
-      <c r="C54" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C56" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="C57" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C58" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>8</v>
       </c>
       <c r="B59" t="s">
+        <v>105</v>
+      </c>
+      <c r="C59" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>8</v>
+      </c>
+      <c r="B60" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" t="s">
         <v>108</v>
       </c>
-      <c r="C59" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>9</v>
-      </c>
-      <c r="B60" t="s">
-        <v>100</v>
-      </c>
-      <c r="C60" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>9</v>
       </c>
       <c r="B61" t="s">
+        <v>99</v>
+      </c>
+      <c r="C61" t="s">
         <v>101</v>
       </c>
-      <c r="C61" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="C63" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9</v>
       </c>
       <c r="B64" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C64" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>9</v>
       </c>
       <c r="B65" t="s">
+        <v>47</v>
+      </c>
+      <c r="C65" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>9</v>
+      </c>
+      <c r="B66" t="s">
         <v>49</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <v>10</v>
-      </c>
-      <c r="B66" t="s">
-        <v>112</v>
-      </c>
-      <c r="C66" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>10</v>
       </c>
       <c r="B67" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>10</v>
+      </c>
+      <c r="B68" t="s">
+        <v>113</v>
+      </c>
+      <c r="C68" t="s">
         <v>114</v>
       </c>
-      <c r="C67" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <v>11</v>
-      </c>
-      <c r="B68" t="s">
-        <v>100</v>
-      </c>
-      <c r="C68" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>11</v>
       </c>
       <c r="B69" t="s">
+        <v>99</v>
+      </c>
+      <c r="C69" t="s">
         <v>101</v>
       </c>
-      <c r="C69" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>48</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="C70" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>117</v>
-      </c>
-      <c r="C71" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C72" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C73" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>12</v>
       </c>
       <c r="B74" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C74" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C75" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>12</v>
       </c>
       <c r="B76" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C76" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C77" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="C78" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>12</v>
+      </c>
+      <c r="B79" t="s">
+        <v>111</v>
+      </c>
+      <c r="C79" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2022 updating module order
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkram02\OneDrive - Emory University\EPI563-Spatial Epi\SpatialEpi-2021\EPI563-SpatialEPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/mkram02_emory_edu/Documents/EPI563-Spatial Epi/EPI563-SpatialEPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_9572770CE0B9746D9A088072FF67B572208C94E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0B4175A-9403-4647-9E26-F6B82C7DF416}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8370"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="23040" windowHeight="8380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,7 +429,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -741,19 +742,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -764,7 +765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -775,7 +776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -786,7 +787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -797,7 +798,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -808,7 +809,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -819,7 +820,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -830,7 +831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -841,7 +842,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -852,7 +853,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -863,7 +864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -874,7 +875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -885,7 +886,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -896,7 +897,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -907,7 +908,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -918,7 +919,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -929,7 +930,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -940,7 +941,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -951,7 +952,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -962,7 +963,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -973,7 +974,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -984,7 +985,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -995,7 +996,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1006,7 +1007,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1017,7 +1018,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4</v>
       </c>
@@ -1039,7 +1040,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -1050,7 +1051,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1061,7 +1062,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1072,7 +1073,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1083,7 +1084,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1094,7 +1095,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>5</v>
       </c>
@@ -1105,7 +1106,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>5</v>
       </c>
@@ -1116,7 +1117,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>5</v>
       </c>
@@ -1127,7 +1128,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>5</v>
       </c>
@@ -1138,7 +1139,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>5</v>
       </c>
@@ -1149,7 +1150,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>5</v>
       </c>
@@ -1160,7 +1161,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>5</v>
       </c>
@@ -1171,9 +1172,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B39" t="s">
         <v>71</v>
@@ -1182,9 +1183,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B40" t="s">
         <v>73</v>
@@ -1193,9 +1194,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
         <v>75</v>
@@ -1204,9 +1205,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
         <v>77</v>
@@ -1215,9 +1216,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
         <v>78</v>
@@ -1226,9 +1227,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B44" t="s">
         <v>81</v>
@@ -1237,9 +1238,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
         <v>48</v>
@@ -1248,9 +1249,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
         <v>83</v>
@@ -1259,9 +1260,9 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
         <v>85</v>
@@ -1270,9 +1271,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
         <v>87</v>
@@ -1281,9 +1282,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B49" t="s">
         <v>91</v>
@@ -1292,9 +1293,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B50" t="s">
         <v>90</v>
@@ -1303,9 +1304,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B51" t="s">
         <v>93</v>
@@ -1314,9 +1315,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B52" t="s">
         <v>95</v>
@@ -1325,9 +1326,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B53" t="s">
         <v>97</v>
@@ -1336,7 +1337,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>8</v>
       </c>
@@ -1347,7 +1348,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>8</v>
       </c>
@@ -1358,7 +1359,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>8</v>
       </c>
@@ -1369,7 +1370,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>8</v>
       </c>
@@ -1380,7 +1381,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>8</v>
       </c>
@@ -1391,7 +1392,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>8</v>
       </c>
@@ -1402,7 +1403,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>8</v>
       </c>
@@ -1413,7 +1414,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>9</v>
       </c>
@@ -1424,7 +1425,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>9</v>
       </c>
@@ -1435,7 +1436,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>9</v>
       </c>
@@ -1446,7 +1447,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>9</v>
       </c>
@@ -1457,7 +1458,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>9</v>
       </c>
@@ -1468,7 +1469,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>9</v>
       </c>
@@ -1479,7 +1480,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>10</v>
       </c>
@@ -1490,7 +1491,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>10</v>
       </c>
@@ -1501,7 +1502,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>11</v>
       </c>
@@ -1512,7 +1513,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>11</v>
       </c>
@@ -1523,7 +1524,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>11</v>
       </c>
@@ -1534,7 +1535,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>11</v>
       </c>
@@ -1545,7 +1546,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>11</v>
       </c>
@@ -1556,7 +1557,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>12</v>
       </c>
@@ -1567,7 +1568,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>12</v>
       </c>
@@ -1578,7 +1579,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>12</v>
       </c>
@@ -1589,7 +1590,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>12</v>
       </c>
@@ -1600,7 +1601,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>12</v>
       </c>
@@ -1611,7 +1612,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Fix PDF  render error and change in syntax for KDE raster CRS
</commit_message>
<xml_diff>
--- a/vocabulary.xlsx
+++ b/vocabulary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/mkram02_emory_edu/Documents/EPI563-Spatial Epi/EPI563-SpatialEPI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/mkram02_emory_edu/Documents/EPI563-Spatial Epi/eBook-EPI563-SpatialEPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_9572770CE0B9746D9A088072FF67B572208C94E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0B4175A-9403-4647-9E26-F6B82C7DF416}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="11_9572770CE0B9746D9A088072FF67B572208C94E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B61D181D-9AC8-4B4D-A28B-5B6FE0A60D0E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="23040" windowHeight="8380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="23040" windowHeight="13660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,12 +439,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -461,8 +467,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1102,7 +1108,7 @@
       <c r="B32" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1504,7 +1510,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B69" t="s">
         <v>99</v>
@@ -1515,7 +1521,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B70" t="s">
         <v>100</v>
@@ -1526,18 +1532,18 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B71" t="s">
         <v>48</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B72" t="s">
         <v>116</v>
@@ -1548,7 +1554,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B73" t="s">
         <v>111</v>
@@ -1558,8 +1564,8 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>12</v>
+      <c r="A74" s="2">
+        <v>11</v>
       </c>
       <c r="B74" t="s">
         <v>118</v>
@@ -1570,7 +1576,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B75" t="s">
         <v>120</v>
@@ -1581,7 +1587,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B76" t="s">
         <v>122</v>
@@ -1592,7 +1598,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B77" t="s">
         <v>124</v>
@@ -1603,7 +1609,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B78" t="s">
         <v>126</v>
@@ -1614,7 +1620,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B79" t="s">
         <v>111</v>

</xml_diff>